<commit_message>
Update Bug Report Sheet
</commit_message>
<xml_diff>
--- a/Manual Testing/Bug Report.xlsx
+++ b/Manual Testing/Bug Report.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdom\OneDrive\Desktop\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdom\OneDrive\Desktop\FP_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29F2982C-11A2-4718-ADE8-1994B868D197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F901C4-0FF7-4C80-B71C-FD2D64F58C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6A41B0FC-DB09-42B3-AB5D-305C53D63295}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{6A41B0FC-DB09-42B3-AB5D-305C53D63295}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product " sheetId="3" r:id="rId1"/>
-    <sheet name="Sign Up" sheetId="1" r:id="rId2"/>
-    <sheet name="Contact Us " sheetId="2" r:id="rId3"/>
+    <sheet name="Home" sheetId="4" r:id="rId1"/>
+    <sheet name="Product " sheetId="3" r:id="rId2"/>
+    <sheet name="Sign Up" sheetId="1" r:id="rId3"/>
+    <sheet name="Contact Us " sheetId="2" r:id="rId4"/>
+    <sheet name="Log out" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="288">
   <si>
     <t>Defect #</t>
   </si>
@@ -846,13 +848,240 @@
   </si>
   <si>
     <t xml:space="preserve"> Product is removed from listings </t>
+  </si>
+  <si>
+    <t>Abdelrahman Ahmed</t>
+  </si>
+  <si>
+    <t>HP01</t>
+  </si>
+  <si>
+    <t>1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully</t>
+  </si>
+  <si>
+    <t>Home page Loads successfully</t>
+  </si>
+  <si>
+    <t>HP02</t>
+  </si>
+  <si>
+    <t>1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5- Press on arrow button next to subscription</t>
+  </si>
+  <si>
+    <t>You have been successfully Subscribed!</t>
+  </si>
+  <si>
+    <t>HP03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5 -Edit to multiple @ symbol in email field
+6- Press on arrow button next to subscription
+</t>
+  </si>
+  <si>
+    <t>System displays error message indicating "Email is invalid "</t>
+  </si>
+  <si>
+    <t>HP04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5 -Edit to special character in email field
+6- Press on arrow button next to subscription</t>
+  </si>
+  <si>
+    <t>HP05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5 -Edit to spaces in email field
+6- Press on arrow button next to subscription</t>
+  </si>
+  <si>
+    <t>HP06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5 -Start email with dot character
+6- Press on arrow button next to subscription</t>
+  </si>
+  <si>
+    <t>HP07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5 -End email with dot character
+6- Press on arrow button next to subscription</t>
+  </si>
+  <si>
+    <t>HP08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5  Edit to consecutive dot in email
+6- Press on arrow button next to subscription
+</t>
+  </si>
+  <si>
+    <t>HP09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5   Leave Email Blank
+6- Press on arrow button next to subscription
+</t>
+  </si>
+  <si>
+    <t>System displays error message indicating "Email is required "</t>
+  </si>
+  <si>
+    <t>HP10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5  Edit to email without @ Symbol
+6- Press on arrow button next to subscription</t>
+  </si>
+  <si>
+    <t>HP11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5  Edit to email without top level domain
+6- Press on arrow button next to subscription
+</t>
+  </si>
+  <si>
+    <t>HP12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5   Edit to email without domain namen
+6- Press on arrow button next to subscription
+</t>
+  </si>
+  <si>
+    <t>HP13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5   Edit to dot character at end of username
+6- Press on arrow button next to subscription
+</t>
+  </si>
+  <si>
+    <t>HP14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5    Edit to space in first character
+6- Press on arrow button next to subscription
+</t>
+  </si>
+  <si>
+    <t>System displays error message indicating "First character cannot have space"</t>
+  </si>
+  <si>
+    <t>HP15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. Verify that home page is visible successfully
+4- scroll down and press on subscription
+5  Edit to Valid Email
+6- Press on arrow button next to subscription</t>
+  </si>
+  <si>
+    <t>System accepts email field</t>
+  </si>
+  <si>
+    <t>HP16</t>
+  </si>
+  <si>
+    <t>1. Launch browser 
+2. Navigate to url 'http://auomationexercise.com'
+3. User on home page</t>
+  </si>
+  <si>
+    <t>Arrow successfully works</t>
+  </si>
+  <si>
+    <t>HP17</t>
+  </si>
+  <si>
+    <t>Not using arrow successfully works</t>
+  </si>
+  <si>
+    <t>LO01</t>
+  </si>
+  <si>
+    <t>1. Launch browser
+2. Navigate to url 'http://automationexercise.com'
+3. Verify that home page is visible successfully
+4. Click on 'Signup / Login' button
+5. Verify 'Login to your account' is visible
+6. Enter correct email address and password
+7. Click 'login' button
+8. Verify that 'Logged in as username' is visible
+9. Click 'Logout' button
+10. Verify that user is navigated to login page</t>
+  </si>
+  <si>
+    <t>System redirects you to signup/login</t>
+  </si>
+  <si>
+    <t>System successfully redirects you to signup/login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -864,13 +1093,6 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -906,20 +1128,66 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -932,8 +1200,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -959,22 +1238,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -982,40 +1298,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{6AFD8DB4-4C1E-4C31-9AD0-701A4B7B706A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1326,11 +1646,611 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27BA5E5F-BF16-436A-AD84-6043E346E21D}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="31.5546875" customWidth="1"/>
+    <col min="8" max="8" width="29.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.3">
+      <c r="A2" s="22">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="135" x14ac:dyDescent="0.3">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.3">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.3">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="150" x14ac:dyDescent="0.3">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="150" x14ac:dyDescent="0.3">
+      <c r="A7" s="22">
+        <v>6</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.3">
+      <c r="A8" s="22">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.3">
+      <c r="A9" s="22">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.3">
+      <c r="A10" s="22">
+        <v>9</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="150" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.3">
+      <c r="A12" s="22">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="165" x14ac:dyDescent="0.3">
+      <c r="A13" s="22">
+        <v>12</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="195" x14ac:dyDescent="0.3">
+      <c r="A14" s="22">
+        <v>13</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="165" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
+        <v>14</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="150" x14ac:dyDescent="0.3">
+      <c r="A16" s="22">
+        <v>15</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.3">
+      <c r="A17" s="22">
+        <v>16</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.3">
+      <c r="A18" s="22">
+        <v>17</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184C71C7-B7BA-4CEA-8CD7-7E010C80C6E4}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,7 +2267,7 @@
     <col min="10" max="10" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="16" customFormat="1" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>160</v>
       </c>
@@ -1377,1046 +2297,1046 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="H4" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I4" s="16" t="s">
+      <c r="H4" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I4" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="H5" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I6" s="16" t="s">
+      <c r="H6" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I7" s="16" t="s">
+      <c r="H7" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I8" s="16" t="s">
+      <c r="H8" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="A9" s="14">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I9" s="16" t="s">
+      <c r="H9" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="H10" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I10" s="16" t="s">
+      <c r="H10" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I10" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
+      <c r="A11" s="14">
         <v>10</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I11" s="16" t="s">
+      <c r="H11" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I11" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="14">
         <v>11</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="14" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
+      <c r="A13" s="14">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="14" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="16">
+      <c r="A14" s="14">
         <v>13</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H14" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I14" s="16" t="s">
+      <c r="H14" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
+      <c r="A15" s="14">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H15" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I15" s="16" t="s">
+      <c r="H15" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I15" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+      <c r="A16" s="14">
         <v>15</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I16" s="16" t="s">
+      <c r="H16" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I16" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="16">
+      <c r="A17" s="14">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H17" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I17" s="16" t="s">
+      <c r="H17" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I17" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="16">
+      <c r="A18" s="14">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H18" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I18" s="16" t="s">
+      <c r="H18" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I18" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="16">
+      <c r="A19" s="14">
         <v>18</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H19" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I19" s="16" t="s">
+      <c r="H19" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I19" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="16">
+      <c r="A20" s="14">
         <v>19</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H20" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I20" s="16" t="s">
+      <c r="H20" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I20" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="16">
+      <c r="A21" s="14">
         <v>20</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H21" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I21" s="16" t="s">
+      <c r="H21" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I21" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="16">
+      <c r="A22" s="14">
         <v>21</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H22" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I22" s="16" t="s">
+      <c r="H22" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I22" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
+      <c r="A23" s="14">
         <v>22</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H23" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I23" s="16" t="s">
+      <c r="H23" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I23" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="16">
+      <c r="A24" s="14">
         <v>23</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H24" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I24" s="16" t="s">
+      <c r="H24" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="16">
+      <c r="A25" s="14">
         <v>24</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G25" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H25" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I25" s="16" t="s">
+      <c r="H25" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="16">
+      <c r="A26" s="14">
         <v>25</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="G26" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H26" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I26" s="16" t="s">
+      <c r="H26" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I26" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="16">
+      <c r="A27" s="14">
         <v>26</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H27" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I27" s="16" t="s">
+      <c r="H27" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I27" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="16">
+      <c r="A28" s="14">
         <v>27</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H28" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I28" s="16" t="s">
+      <c r="H28" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I28" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="16">
+      <c r="A29" s="14">
         <v>28</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="G29" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H29" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I29" s="16" t="s">
+      <c r="H29" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I29" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="16">
+      <c r="A30" s="14">
         <v>29</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="G30" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H30" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I30" s="16" t="s">
+      <c r="H30" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I30" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="16">
+      <c r="A31" s="14">
         <v>30</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G31" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H31" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I31" s="16" t="s">
+      <c r="H31" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I31" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="16">
+      <c r="A32" s="14">
         <v>31</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="H32" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I32" s="16" t="s">
+      <c r="H32" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I32" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="16">
+      <c r="A33" s="14">
         <v>32</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="H33" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I33" s="16" t="s">
+      <c r="H33" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I33" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="16">
+      <c r="A34" s="14">
         <v>33</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="H34" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I34" s="16" t="s">
+      <c r="H34" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I34" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="16">
+      <c r="A35" s="14">
         <v>34</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="G35" s="16" t="s">
+      <c r="G35" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="H35" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I35" s="16" t="s">
+      <c r="H35" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I35" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="16">
+      <c r="A36" s="14">
         <v>35</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="G36" s="16" t="s">
+      <c r="G36" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="H36" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I36" s="16" t="s">
+      <c r="H36" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I36" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="16">
+      <c r="A37" s="14">
         <v>36</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F37" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G37" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="H37" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="I37" s="16" t="s">
+      <c r="H37" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I37" s="14" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2425,359 +3345,360 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27361D1-68B5-4F7B-80C0-1E316C037312}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="42.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9" s="13" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="H5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="H6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="H10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="34.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFD6871-8805-48F9-A3F1-615ACA6E8F20}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2794,836 +3715,926 @@
     <col min="10" max="10" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" s="17" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="I4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="I5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="4" t="s">
+      <c r="I6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="102" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="122.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="4" t="s">
+      <c r="I11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="4" t="s">
+      <c r="I12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" s="4" t="s">
+      <c r="I13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="I14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="4" t="s">
+      <c r="I15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="I16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="4" t="s">
+      <c r="I17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="4" t="s">
+      <c r="I18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="122.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="4" t="s">
+      <c r="I19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="122.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="4" t="s">
+      <c r="I20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J21" s="4" t="s">
+      <c r="I21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" s="4" t="s">
+      <c r="I22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="122.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J23" s="4" t="s">
+      <c r="I23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="122.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J24" s="4" t="s">
+      <c r="I24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="122.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J25" s="4" t="s">
+      <c r="I25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="122.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>49</v>
+      <c r="I26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4460C01C-2481-48C6-9F21-EFE6515E6CBA}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="47.77734375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="39" style="19" customWidth="1"/>
+    <col min="8" max="8" width="47.21875" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="165" x14ac:dyDescent="0.3">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>